<commit_message>
Big update -- halfway through
</commit_message>
<xml_diff>
--- a/data/Orcus - Classes.xlsx
+++ b/data/Orcus - Classes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Obsidian\Tabletop games\d20 System or D&amp;D-esque\2021 Orcus - 4E clone\GitHub\orcus\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5D5D26-997A-40DE-892F-9B90BE8B49D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D130C6C-A406-4049-90C2-02AC198076EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{190BB917-E992-4FE1-9680-9C1683F26666}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="233">
   <si>
     <t>Name</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Dualclass</t>
   </si>
   <si>
-    <t>Specialist Wizard</t>
-  </si>
-  <si>
     <t>Arcane</t>
   </si>
   <si>
@@ -164,26 +161,9 @@
     <t>Arcana</t>
   </si>
   <si>
-    <t>Arcane Overflow</t>
-  </si>
-  <si>
-    <t>Encounter attack powers from your class gain the following Miss entry if they do not have one:
-*Miss:* Half damage, and if a hit would have imposed a condition, the target experiences the following (same duration). 
-* *Blinded:* -2 to hit.
-* *Controlled:* Dazed.
-* *Immobile:* Slowed.
-* *Persistent damage 10 or more:* Persistent damage 5.
-* *Stunned:* Dazed.
-* *Weakened:* -4 to damage.
-* *Unwilling movement 3 or more:* Unwilling movement of the same variety 1.</t>
-  </si>
-  <si>
     <t>Magical Training</t>
   </si>
   <si>
-    <t>You gain the Athame, Alchemist or Incantation Caster feat (your choice).</t>
-  </si>
-  <si>
     <t>Cantrips</t>
   </si>
   <si>
@@ -193,20 +173,6 @@
     <t>Intelligence</t>
   </si>
   <si>
-    <t>Spells of Ice and Fire, Cup of Brimstone, Puppeteer's Pull</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You belong to a particular school of magic. Choose one at character creation. 
-* **Conjurer:** When an encounter ends and you have one or more daily powers with the Summon keyword still active, those daily powers are not expended. However, if you use them again, the summoned creatures appear in the exact state they were when their last summoning ended (current HP, conditions, etc). If you complete a long rest, all your daily powers reset and if you use them from then on a "fresh" creature will be summoned. Your secondary ability is Constitution.
-* **Enchanter:** Once per encounter, when you place a save-ends condition on a creature, you may choose to give them a -2 penalty to saves to end that particular condition. Your secondary ability is Charisma. 
-* **Evoker:** Choose a flux energy (fire, cold, acid, thunder or lightning) at character creation. While that energy is your flux energy, some powers you use are more effective (as indicated by the Elemental Attunement line). You can change your flux energy as a swift action. Your secondary ability is Dexterity. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">You belong to the Specialist Wizard class (along with any other classes that you belong to), and gain the following benefits:
-* You are proficient with one of the following: orb, staff, wand, rod or book.
-* Choose one at-will 1st-level attack power from a Specialist Wizard class discipline. It is an encounter power for you. </t>
-  </si>
-  <si>
     <t>Mageblade</t>
   </si>
   <si>
@@ -222,22 +188,10 @@
     <t>Simple melee, martial melee; simple ranged</t>
   </si>
   <si>
-    <t>See Special Bond feature.</t>
-  </si>
-  <si>
     <t>Arcana, Acrobatics, Athletics, Diplomacy, Endure, History, Insight, Intimidate</t>
   </si>
   <si>
-    <t>Mageblade's Sigil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use the *mageblade's sigil* power. </t>
-  </si>
-  <si>
     <t>Athame</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You have the Athame feat for the weapon type that your particular weapon belongs to. For example, if your particular weapon is a *+1 longsword*, you have the Athame (longsword) feat. This changes if your Special Bond changes. </t>
   </si>
   <si>
     <t>Key Weapon</t>
@@ -250,9 +204,6 @@
   </si>
   <si>
     <t>Shimmering Shield</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If you have a spare hand (not carrying a shield, wielding a two-handed weapon, etc.), you receive a +2 shield bonus to AC. </t>
   </si>
   <si>
     <t>Elemental Flux, Veiled Moon</t>
@@ -265,11 +216,6 @@
 * **Rush Specialist:** Your secondary ability is Strength. You can use the *beacon sigil* power.</t>
   </si>
   <si>
-    <t>You belong to the Mageblade class (along with any other classes that you belong to), and gain the following benefits:
-* You can use *mageblade's sigil* once per encounter. 
-* Choose one of *beacon sigil*, *blurring sigil*, *fiery sigil* or *vortex sigil*. You can use that power once per encounter.</t>
-  </si>
-  <si>
     <t>Crusader</t>
   </si>
   <si>
@@ -307,9 +253,6 @@
     <t>You can use the *infuse with life* power twice per encounter.</t>
   </si>
   <si>
-    <t>You gain the Athame, Alchemist, Cantrip Master or Incantation Caster feat (your choice).</t>
-  </si>
-  <si>
     <t>Action Recharge</t>
   </si>
   <si>
@@ -317,9 +260,6 @@
   </si>
   <si>
     <t>Wisdom</t>
-  </si>
-  <si>
-    <t>Angel's Trumpet</t>
   </si>
   <si>
     <t xml:space="preserve">Choose one kit that begins with "Worships …". You gain the benefits of that kit at the appropriate levels, including the associated discipline. This is in addition to any other kits you may have. 
@@ -349,18 +289,6 @@
     <t>Bluff or Diplomacy</t>
   </si>
   <si>
-    <t>Double Your Efforts</t>
-  </si>
-  <si>
-    <t>Once per round, you can use a swift action and spend a recovery. You gain no hit points; instead, you gain a standard action you must use before the end of your next turn.</t>
-  </si>
-  <si>
-    <t>Wrong Place - Wrong Time</t>
-  </si>
-  <si>
-    <t>You gain the *wrong place-wrong time* power. As a free action, you can discard any unused encounter attack power and gain a use of *wrong place-wrong time*. You can only use *wrong place-wrong time* once per turn.</t>
-  </si>
-  <si>
     <t>Character Actor</t>
   </si>
   <si>
@@ -373,15 +301,6 @@
     <t>Last Laugh</t>
   </si>
   <si>
-    <t xml:space="preserve">Choose one at character creation.
-* **Clown:** Any targets you have marked suffer an additional -2 penalty to attack rolls for any attack that does not include you. Your secondary ability is Dexterity.  
-* **Fool:** Creatures subject to an effect you caused (e.g. a condition or persistent damage) suffer a -2 penalty to attacks against you. Your secondary ability is Wisdom. </t>
-  </si>
-  <si>
-    <t>You belong to the Jester class (along with any other classes that you belong to), and gain the following benefits:
-* Once per encounter, you can use the *wrong place—wrong time* power.</t>
-  </si>
-  <si>
     <t>Guard</t>
   </si>
   <si>
@@ -397,31 +316,10 @@
     <t>Athletics, Endure, Heal, Intimidate, Streetsmarts</t>
   </si>
   <si>
-    <t>Guard's Challenge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When you hit or miss a target with an attack, you may mark them until the end of your next turn. </t>
-  </si>
-  <si>
-    <t>Punish Cowardice</t>
-  </si>
-  <si>
-    <t>*Trigger:* An adjacent creature you have marked shifts or makes an attack that does not include you.
-*Action:* Immediate (Counter)
-*Effect:* Make a basic melee attack against the triggering creature.</t>
-  </si>
-  <si>
     <t>Veteran Opportunist</t>
   </si>
   <si>
     <t>Add your Wisdom modifier to your attack rolls when making opportunity attacks.</t>
-  </si>
-  <si>
-    <t>Block Retreat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Trigger:* A creature is hit by your opportunity attack, and the opportunity attack was provoked by movement.
-*Effect:* Their movement stops for this action. They may attempt to move again using another action, if applicable. </t>
   </si>
   <si>
     <t>Strength</t>
@@ -435,35 +333,16 @@
 * **Protection:** Your secondary ability is Dexterity OR Wisdom (your choice). You get a +1 bonus on attack rolls with one-handed weapons.</t>
   </si>
   <si>
-    <t xml:space="preserve">You belong to the Guard class (along with any other classes that you belong to), and gain the following benefits:
-* Once per encounter, you get a +1 bonus on an attack roll. All targets of the attack (whether you hit them or not) are marked until the end of your next turn. </t>
-  </si>
-  <si>
     <t>Commander</t>
   </si>
   <si>
     <t>Cloth, leather, hide, chainmail, scale; light shields</t>
   </si>
   <si>
-    <t>Simple melee, martial melee; simple ranged.</t>
-  </si>
-  <si>
     <t>Athletics, Diplomacy, Endure, Heal, History, Intimidate, Religion</t>
   </si>
   <si>
-    <t>Stratagem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The first time in an encounter that you use a power, you gain a bonus based on the discipline. Once this bonus is in place, using a power from a different discipline will change which bonus is granted.
-**Golden Lion:** Allies that are adjacent to you get a +1 bonus on attack rolls.
-**Angel's Trumpet:** Allies that are adjacent to you get resistance to all damage 2. *Level 11:* Resistance to all damage 4. *Level 21:* Resistance to all damage 6. 
-**Any other discipline:** Allies that are adjacent to you get a +1 bonus on Fortitude, Reflex and Will defenses. </t>
-  </si>
-  <si>
     <t>Lift Spirits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use the *lift spirits* power two times each encounter. *Level 16:* Three times per encounter. </t>
   </si>
   <si>
     <t>Armament</t>
@@ -475,16 +354,6 @@
 * Proficiency with two exotic melee weapons of your choice. </t>
   </si>
   <si>
-    <t>Angel's Trumpet, Golden Lion</t>
-  </si>
-  <si>
-    <t>Choose one at character creation. 
-* **React to Ill Fortune:** If an ally within 5 misses with an attack, they can shift 1 as a free action. Your secondary ability is Intelligence. 
-* **React to Good Fortune:** If an ally within 5 makes a critical hit, choose an ally within 5. They get a +2 bonus on their next attack roll (if they use it before the end of your next turn). Your secondary ability is Strength. 
-* **React to Despair:** Allies within 5 gain a +1 bonus to their saving throws for every saving throw that they have failed in that turn. Your secondary ability is Intelligence. 
-* **React to Treachery:** Allies within 5 get a +1 bonus to all defenses against attacks that have combat advantage against them. Your secondary ability is Dexterity.</t>
-  </si>
-  <si>
     <t xml:space="preserve">You belong to the Commander class (along with any other classes that you belong to), and gain the following benefits:
 * You can use *lifting words* once per encounter. </t>
   </si>
@@ -536,19 +405,6 @@
     <t>Dexterity</t>
   </si>
   <si>
-    <t>Rapier's Point, Blades in the Dark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose one at character creation. 
-* **Forceful Swashbuckler:** Your secondary ability is Strength. Once per turn, when you shift, you can pull an adjacent enemy 1 at one point during your movement. 
-* **Goading Swashbuckler:** Your secondary ability is Charisma. Your triumphant strike does additional damage equal to your Charisma modifier when you attack a marked enemy. </t>
-  </si>
-  <si>
-    <t>You belong to the Swashbuckler class (along with any other classes that you belong to), and gain the following benefits:
-* When you hit an enemy with a melee attack, you gain momentum. When you are hit by any kind of attack, you lose momentum. Momentum has no effect on its own, but it is required for your Triumphant Strike feature and is referenced by some powers.
-* Once per encounter, you can use the Swashbuckler's Triumphant Strike feature (noting that it requires momentum to use).</t>
-  </si>
-  <si>
     <t>Reaper</t>
   </si>
   <si>
@@ -574,10 +430,6 @@
   </si>
   <si>
     <t>Spirit Entreaty</t>
-  </si>
-  <si>
-    <t>You gain the ability to entreat the spirits for a favour. You start with three such effects: *grasping vines*, *spirit's prank* and *unleashed spirit*.
-When you use your Spirit Entreaty, you choose which effect to create. You can use Spirit Entreaty once per encounter, however many powers you learn that are usable through Spirit Entreaty (although see Action Recharge).</t>
   </si>
   <si>
     <t xml:space="preserve">When you spend an action point, you recover the use of Spirit Entreaty for the encounter. </t>
@@ -612,6 +464,264 @@
   </si>
   <si>
     <t>Wild Gift</t>
+  </si>
+  <si>
+    <t>Favored Terrain</t>
+  </si>
+  <si>
+    <t>Constitution</t>
+  </si>
+  <si>
+    <t>Red in Tooth and Claw, Strong Bidding, Frontline Fighting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose one at character creation. Note that rampage powers do not necessarily have to target the creature that you hit with the attack that triggered the rampage power. 
+* **Watchful:** Your secondary ability is Wisdom. You gain the *fearful rampage* power. 
+* **Companionable:** Your secondary ability is Charisma. You gain the *companion rampage* power. 
+* **Swift:** Your secondary ability is Dexterity. You gain the *swift rampage* power. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You belong to the Sylvan class (along with any other classes that you belong to), and gain the following benefit:
+* Choose a rampage power. Once per encounter, you can use that power. </t>
+  </si>
+  <si>
+    <t>Vanguard</t>
+  </si>
+  <si>
+    <t>Cloth, leather, hide, chainmail, scale</t>
+  </si>
+  <si>
+    <t>Distinct Advantage</t>
+  </si>
+  <si>
+    <t>You gain the *distinct advantage* power. As a free action, you can expend an unused encounter attack power and gain a use of *distinct advantage*. You can only use *distinct advantage* once per turn.</t>
+  </si>
+  <si>
+    <t>Fighting Form</t>
+  </si>
+  <si>
+    <t>You gain the Unarmed Combat feat. Your natural weapons gain the off-hand property. You add your proficiency and enhancement bonus with unarmed attacks to all grab attempts. You also gain one additional martial training feat you are eligible for.</t>
+  </si>
+  <si>
+    <t>Impact Force</t>
+  </si>
+  <si>
+    <t>The damage die of your unarmed attacks increases by one step (1d4 &gt; 1d6 &gt; 1d8 &gt; 1d10 &gt; 1d12 &gt; 2d6 &gt; d28 &gt; 2d10). This is cumulative with effects that do the same.</t>
+  </si>
+  <si>
+    <t>Mobile Stance</t>
+  </si>
+  <si>
+    <t>As a swift action, you can shift 1 square as long as the shift brings you closer to your closest enemy. While you are wearing light armor or no armor, gain a +1 bonus to attack rolls against adjacent targets.</t>
+  </si>
+  <si>
+    <t>Frontline Fighting, Art of War</t>
+  </si>
+  <si>
+    <t>Rod, wand</t>
+  </si>
+  <si>
+    <t>Harbinger</t>
+  </si>
+  <si>
+    <t>Arcana, Bluff, History, Insight, Intimidate, Religion, Streetsmarts, Sleight of Hand</t>
+  </si>
+  <si>
+    <t>Dark Claim</t>
+  </si>
+  <si>
+    <t>You reach out with sorcerous malice, marking foes as your own. 
+As a swift action once per turn, you may Claim the nearest opponent that you can see (including with special senses such as blindsense or tremorsense). You may Claim any number of creatures. The Claim ends after five minutes or when the creature falls to 0 HP. 
+Your attacks and attacks of your summoned creatures against targets you have Claimed do +1d6 damage (*Level 11:* +2d6; *Level 21:* +3d6).</t>
+  </si>
+  <si>
+    <t>Precise Shot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You get a +1 bonus on attack rolls against enemies for which you are the nearest (or tied nearest) enemy. </t>
+  </si>
+  <si>
+    <t>Elusive Shadow</t>
+  </si>
+  <si>
+    <t>Your unnatural alacrity protects you from harm as you shy away from whirling blades and streaking spells alike.
+If you move 3 or more squares during your turn, you gain concealment until the end of your next turn.</t>
+  </si>
+  <si>
+    <t>Cup of Brimstone, Veiled Moon</t>
+  </si>
+  <si>
+    <t>Demonologist, Fey Changeling, Starchild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose one at character creation.  Based on your talent, you have a benefit that triggers every time a creature you have Claimed is reduced to 0 HP.
+* *Omenwalk (Fey Changeling):* Free action. You teleport 3. Also, your secondary ability is Charisma. 
+* *Quick and the Dead (Demonologist):* You gain your level in temporary HP. Also, your secondary ability is Constitution. 
+* *Accursed Will (Starchild):* Until the end of your next turn, you get a floating +1 bonus to any d20 roll you make. These floating bonuses stack, but you only get each bonus to one roll. Also, your secondary ability is Intelligence. </t>
+  </si>
+  <si>
+    <t>Shaper</t>
+  </si>
+  <si>
+    <t>Phrenic</t>
+  </si>
+  <si>
+    <t>Acrobatics, Arcana, Athletics, Diplomacy, Dungeoneering, History, Insight, Nature, Religion</t>
+  </si>
+  <si>
+    <t>Dream Residue</t>
+  </si>
+  <si>
+    <t>You have the dream residue* at-will utility power.
+You can use an *dream residue* zone as the origin square for any Phrenic powers that you use, but after you do so that particular *dream residue* disappears.</t>
+  </si>
+  <si>
+    <t>Lingering Punishment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whenever a creature successfully saves to end a condition or persistent damage you imposed on them, you can spend your *psi focus* to give them an aftereffect based on your focus. An aftereffect applies after a successful saving throw against the initial effect. 
+* **Rod:** 1d6 points of fire damage. *Level 11: 2d6 points of fire damage. *Level 21:* 3d6 points of fire damage.
+* **Orb:** The target makes a save. If they fail, they are dazed (save ends).  
+* **Staff:** Shunt 1.
+* **Wand:** The target makes a save. If they fail, they fall prone. 
+* **Book:** The target makes a save. If they fail, they are slowed (save ends). </t>
+  </si>
+  <si>
+    <t>Psi Focus</t>
+  </si>
+  <si>
+    <t>You have access to psi focus, a heightened state of mental and emotional clarity, that you can utilize to augment powers with the Augmentable keyword. This psi focus, once used, must refresh, much like how certain monsters have powers that refresh at the beginning of their turn on a successful roll. Psi focus works in the exact same way, refreshing on a roll of 5 or 6.  
+&gt; #### Psi Focus
+&gt; *Utilizing your phrenic power, you heighten a power or ability beyond what others could fathom.*
+&gt; **At-Will** **Free Action**
+&gt; **Channels Godmind Utility Feature** ● **Phrenic**
+&gt; **Self** 
+&gt; **Effect:** When using an Augmentable power, you activate the effect noted under the Augment: line.</t>
+  </si>
+  <si>
+    <t>Focus Surges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At level 1, you have one focus surge. This increases to two at level 3, three at level 7, four at level 17 and five at level 27. As a swift action, you can spend a focus surge to regain your *psi focus*. </t>
+  </si>
+  <si>
+    <t>Perchance to Dream, Invisible Cities</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Defense Bonuses</t>
+  </si>
+  <si>
+    <t>Myrmidon</t>
+  </si>
+  <si>
+    <t>Swordsaint</t>
+  </si>
+  <si>
+    <t>Wilder</t>
+  </si>
+  <si>
+    <t>Striker/Defender</t>
+  </si>
+  <si>
+    <t>+1 Fortitude, +1 Will</t>
+  </si>
+  <si>
+    <t>Captain</t>
+  </si>
+  <si>
+    <t>Impudent Flourish</t>
+  </si>
+  <si>
+    <t>You do not provoke opportunity attacks from creatures you have attacked this turn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose one at character creation.
+* **Clown:** Creatures you have marked suffer an additional -2 penalty to attack rolls for any attack that does not include you. Your secondary ability is Dexterity.  
+* **Fool:** Creatures that are marked, not by you, suffer a -2 penalty to attack rolls against you (this stacks with the marked penalty, if any). Your secondary ability is Wisdom. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you have a spare hand (not carrying a shield, wielding a two-handed weapon, holding a focus, etc.), you receive a +2 shield bonus to AC. </t>
+  </si>
+  <si>
+    <t>Combat Dominance</t>
+  </si>
+  <si>
+    <t>You can choose to emit an aura 1 of combat dominance. While you do so, creatures in the aura who are not marked by anyone else are marked by you. A creature that leaves your aura is no longer marked.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use the *lift spirits* power two times each encounter.  
+*Level 16:* Three times per encounter. </t>
+  </si>
+  <si>
+    <t>Rook by Jared von Hindman</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Art Link</t>
+  </si>
+  <si>
+    <t>pics\rook.jpg</t>
+  </si>
+  <si>
+    <t>Art Zoom</t>
+  </si>
+  <si>
+    <t>Choose one at character creation. 
+* **Stormtrooper Tactics:** Once per turn, an ally that is the target of one of your powers can shift 1 as a free action. Your secondary ability is Dexterity. 
+* **Siege Tactics:** Once per turn, an ally that is the target of one of your powers receives temporary hit points equal to your Wisdom modifier (double at level 11, triple at level 21). Your secondary ability is Wisdom. 
+* **Resilience Tactics:** Once per turn, an ally that is the target of one of your powers immediately makes a saving throw against one save ends condition they are subject to. Your secondary ability is Intelligence. 
+* **Inspiring Tactics:** Once per turn, an ally that is the target of one of your powers receives a +2 power bonus to their next attack roll. Your secondary ability is Strength.</t>
+  </si>
+  <si>
+    <t>Charlene by Justin Nichol</t>
+  </si>
+  <si>
+    <t>pics\Charlene.png</t>
+  </si>
+  <si>
+    <t>pics\WarriorBIG (1).jpg</t>
+  </si>
+  <si>
+    <t>Warrior by Sarah Carney</t>
+  </si>
+  <si>
+    <t>pics\Vera.png</t>
+  </si>
+  <si>
+    <t>Vera by Justin Nichols</t>
+  </si>
+  <si>
+    <t>pics\Flashing Ray Color.png</t>
+  </si>
+  <si>
+    <t>Flashing Ray by Crystal Frasier</t>
+  </si>
+  <si>
+    <t>Magician</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You belong to the Magician class (along with any other classes that you belong to), and gain the following benefits:
+* You are proficient with one of the following: orb, staff, wand, rod or book.
+* Choose one at-will 1st-level attack power from a Magician class discipline. It is an encounter power for you. </t>
+  </si>
+  <si>
+    <t>Rapier’s Point, Blades in the Dark</t>
+  </si>
+  <si>
+    <t>You belong to the Swashbuckler class (along with any other classes that you belong to), and gain the following benefits:
+* When you hit an enemy with a melee attack, you gain momentum. When you are hit by any kind of attack, you lose momentum. Momentum has no effect on its own, but it is required for your Triumphant Strike feature and is referenced by some powers.
+* Once per encounter, you can use the Swashbuckler’s Triumphant Strike feature (noting that it requires momentum to use).</t>
   </si>
   <si>
     <t xml:space="preserve">Choose one of the following.
@@ -624,8 +734,8 @@
 * You can give up actions to command the animal companion, in which case it gets to take the same actions. For example, you can give up your standard action in order for the animal companion to take a standard action. You can also use an immediate action in order for the animal companion to make an opportunity attack (if eligible to do so). 
 * If you are incapacitated or not present, your animal companion gets its full complement of actions without needing to be "commanded". However, it acts like the animal it is: loyally but with limited intelligence. 
 *Stats and Combat*
-* The animal companion's level is equal to your own.
-* The animal companion's maximum HP are equal to your staggered value. 
+* The animal companion’s level is equal to your own.
+* The animal companion’s maximum HP are equal to your staggered value. 
 * Your animal companion has no recoveries of its own, but can use yours. 
 * Whenever you have the chance to spend a recovery to heal, you can spend a second recovery to heal your animal companion your recovery value. 
 * When your animal companion drops to 0 hit points, it disappears, leaving behind no physical form. It reappears after your next long rest, at full HP. 
@@ -637,188 +747,100 @@
 * The animal companion is a bright, sensitive animal, but nonetheless has animal-level intelligence. </t>
   </si>
   <si>
-    <t>Favored Terrain</t>
+    <t>You belong to the Harbinger class (along with any other classes that you belong to), and gain the following benefits:
+* You gain one at-will attack power from the Harbinger’s class disciplines as an encounter power.
+* You gain proficiency in rods, wands and daggers (see Athame feat) for the use of Warlock and Harbinger powers only.</t>
+  </si>
+  <si>
+    <t>Angel’s Trumpet, Golden Lion</t>
+  </si>
+  <si>
+    <t>Angel’s Trumpet</t>
+  </si>
+  <si>
+    <t>Mageblade’s Sigil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use the *mageblade’s sigil* power. </t>
+  </si>
+  <si>
+    <t>You belong to the Mageblade class (along with any other classes that you belong to), and gain the following benefits:
+* You can use *mageblade’s sigil* once per encounter. 
+* Choose one of *beacon sigil*, *blurring sigil*, *fiery sigil* or *vortex sigil*. You can use that power once per encounter.</t>
+  </si>
+  <si>
+    <t>You gain the ability to entreat the spirits for a favour. You start with three such effects: *grasping vines*, *spirit’s prank* and *unleashed spirit*.
+When you use your Spirit Entreaty, you choose which effect to create. You can use Spirit Entreaty once per encounter, however many powers you learn that are usable through Spirit Entreaty (although see Action Recharge).</t>
+  </si>
+  <si>
+    <t>Spells of Ice and Fire, Cup of Brimstone, Puppeteer’s Pull</t>
+  </si>
+  <si>
+    <t>You gain the Athame, Cantrip Master or Incantation Caster feat (your choice).</t>
+  </si>
+  <si>
+    <t>You belong to the Guard class (along with any other classes that you belong to), and gain the following benefits:
+* Once per encounter, as a free action, you gain the Combat Dominance feature until the end of your next turn.</t>
+  </si>
+  <si>
+    <t>Savvy Combatant</t>
+  </si>
+  <si>
+    <t>You gain the *punish cowardice* and *block retreat* powers.</t>
+  </si>
+  <si>
+    <t>Clever Fellow</t>
+  </si>
+  <si>
+    <t>You gain the *hasty retreat* and *general confusion* powers.</t>
+  </si>
+  <si>
+    <t>You belong to the Jester class (along with any other classes that you belong to), and gain the following benefits:
+* Once per encounter, you can use the *hasty retreat* power. 
+* Once per encounter, you can use the *general confusion* power.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have the Athame feat for the weapon type that your key weapon belongs to. For example, if your key weapon is a *+1 longsword*, you have the Athame (longsword) feat. This changes if your Special Bond changes. </t>
+  </si>
+  <si>
+    <t>See Athame feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose one at character creation. 
+* **Forceful Swashbuckler:** Your secondary ability is Strength. Once per turn, when you shift, you can shunt an adjacent enemy 1 at one point during your movement. 
+* **Goading Swashbuckler:** Your secondary ability is Charisma. Your triumphant strike does additional damage equal to your Charisma modifier when you attack a marked enemy. </t>
   </si>
   <si>
     <t xml:space="preserve">After spending a week or more in a particular terrain, you can set it as your Favored Terrain. After spending a week or more in a different terrain, you can change your Favored Terrain.
-* **Arctic:** You gain the Ice Stride feature and a +2 bonus to Endure. 
-* **Forest or Heath:** You gain the Woodland Stride feature and a +2 bonus to Nature.
-* **Marshes:** You gain the Swamp Stride feature and a +2 bonus to Athletics. 
-* **Underground or Mountains:** You gain the Stone Stride feature and a +2 bonus to Dungeoneering. </t>
-  </si>
-  <si>
-    <t>Constitution</t>
-  </si>
-  <si>
-    <t>Red in Tooth and Claw, Strong Bidding, Frontline Fighting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose one at character creation. Note that rampage powers do not necessarily have to target the creature that you hit with the attack that triggered the rampage power. 
-* **Watchful:** Your secondary ability is Wisdom. You gain the *fearful rampage* power. 
-* **Companionable:** Your secondary ability is Charisma. You gain the *companion rampage* power. 
-* **Swift:** Your secondary ability is Dexterity. You gain the *swift rampage* power. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">You belong to the Sylvan class (along with any other classes that you belong to), and gain the following benefit:
-* Choose a rampage power. Once per encounter, you can use that power. </t>
-  </si>
-  <si>
-    <t>Vanguard</t>
-  </si>
-  <si>
-    <t>Cloth, leather, hide, chainmail, scale</t>
-  </si>
-  <si>
-    <t>Distinct Advantage</t>
-  </si>
-  <si>
-    <t>You gain the *distinct advantage* power. As a free action, you can expend an unused encounter attack power and gain a use of *distinct advantage*. You can only use *distinct advantage* once per turn.</t>
-  </si>
-  <si>
-    <t>Fighting Form</t>
-  </si>
-  <si>
-    <t>You gain the Unarmed Combat feat. Your natural weapons gain the off-hand property. You add your proficiency and enhancement bonus with unarmed attacks to all grab attempts. You also gain one additional martial training feat you are eligible for.</t>
-  </si>
-  <si>
-    <t>Impact Force</t>
-  </si>
-  <si>
-    <t>The damage die of your unarmed attacks increases by one step (1d4 &gt; 1d6 &gt; 1d8 &gt; 1d10 &gt; 1d12 &gt; 2d6 &gt; d28 &gt; 2d10). This is cumulative with effects that do the same.</t>
-  </si>
-  <si>
-    <t>Mobile Stance</t>
-  </si>
-  <si>
-    <t>As a swift action, you can shift 1 square as long as the shift brings you closer to your closest enemy. While you are wearing light armor or no armor, gain a +1 bonus to attack rolls against adjacent targets.</t>
-  </si>
-  <si>
-    <t>Frontline Fighting, Art of War</t>
-  </si>
-  <si>
-    <t>Rod, wand</t>
-  </si>
-  <si>
-    <t>Harbinger</t>
-  </si>
-  <si>
-    <t>Arcana, Bluff, History, Insight, Intimidate, Religion, Streetsmarts, Sleight of Hand</t>
-  </si>
-  <si>
-    <t>Dark Claim</t>
-  </si>
-  <si>
-    <t>You reach out with sorcerous malice, marking foes as your own. 
-As a swift action once per turn, you may Claim the nearest opponent that you can see (including with special senses such as blindsense or tremorsense). You may Claim any number of creatures. The Claim ends after five minutes or when the creature falls to 0 HP. 
-Your attacks and attacks of your summoned creatures against targets you have Claimed do +1d6 damage (*Level 11:* +2d6; *Level 21:* +3d6).</t>
-  </si>
-  <si>
-    <t>Precise Shot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You get a +1 bonus on attack rolls against enemies for which you are the nearest (or tied nearest) enemy. </t>
-  </si>
-  <si>
-    <t>Elusive Shadow</t>
-  </si>
-  <si>
-    <t>Your unnatural alacrity protects you from harm as you shy away from whirling blades and streaking spells alike.
-If you move 3 or more squares during your turn, you gain concealment until the end of your next turn.</t>
-  </si>
-  <si>
-    <t>Cup of Brimstone, Veiled Moon</t>
-  </si>
-  <si>
-    <t>Demonologist, Fey Changeling, Starchild</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose one at character creation.  Based on your talent, you have a benefit that triggers every time a creature you have Claimed is reduced to 0 HP.
-* *Omenwalk (Fey Changeling):* Free action. You teleport 3. Also, your secondary ability is Charisma. 
-* *Quick and the Dead (Demonologist):* You gain your level in temporary HP. Also, your secondary ability is Constitution. 
-* *Accursed Will (Starchild):* Until the end of your next turn, you get a floating +1 bonus to any d20 roll you make. These floating bonuses stack, but you only get each bonus to one roll. Also, your secondary ability is Intelligence. </t>
-  </si>
-  <si>
-    <t>You belong to the Harbinger class (along with any other classes that you belong to), and gain the following benefits:
-* You gain one at-will attack power from the Harbinger's class disciplines as an encounter power.
-* You gain proficiency in rods, wands and daggers (see Athame feat) for the use of Warlock and Harbinger powers only.</t>
-  </si>
-  <si>
-    <t>Shaper</t>
-  </si>
-  <si>
-    <t>Phrenic</t>
-  </si>
-  <si>
-    <t>Acrobatics, Arcana, Athletics, Diplomacy, Dungeoneering, History, Insight, Nature, Religion</t>
-  </si>
-  <si>
-    <t>Dream Residue</t>
-  </si>
-  <si>
-    <t>You have the dream residue* at-will utility power.
-You can use an *dream residue* zone as the origin square for any Phrenic powers that you use, but after you do so that particular *dream residue* disappears.</t>
-  </si>
-  <si>
-    <t>Lingering Punishment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whenever a creature successfully saves to end a condition or persistent damage you imposed on them, you can spend your *psi focus* to give them an aftereffect based on your focus. An aftereffect applies after a successful saving throw against the initial effect. 
-* **Rod:** 1d6 points of fire damage. *Level 11: 2d6 points of fire damage. *Level 21:* 3d6 points of fire damage.
-* **Orb:** The target makes a save. If they fail, they are dazed (save ends).  
-* **Staff:** Shunt 1.
-* **Wand:** The target makes a save. If they fail, they fall prone. 
-* **Book:** The target makes a save. If they fail, they are slowed (save ends). </t>
-  </si>
-  <si>
-    <t>Psi Focus</t>
-  </si>
-  <si>
-    <t>You have access to psi focus, a heightened state of mental and emotional clarity, that you can utilize to augment powers with the Augmentable keyword. This psi focus, once used, must refresh, much like how certain monsters have powers that refresh at the beginning of their turn on a successful roll. Psi focus works in the exact same way, refreshing on a roll of 5 or 6.  
-&gt; #### Psi Focus
-&gt; *Utilizing your phrenic power, you heighten a power or ability beyond what others could fathom.*
-&gt; **At-Will** **Free Action**
-&gt; **Channels Godmind Utility Feature** ● **Phrenic**
-&gt; **Self** 
-&gt; **Effect:** When using an Augmentable power, you activate the effect noted under the Augment: line.</t>
-  </si>
-  <si>
-    <t>Focus Surges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At level 1, you have one focus surge. This increases to two at level 3, three at level 7, four at level 17 and five at level 27. As a swift action, you can spend a focus surge to regain your *psi focus*. </t>
-  </si>
-  <si>
-    <t>Perchance to Dream, Invisible Cities</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Defense Bonuses</t>
-  </si>
-  <si>
-    <t>Myrmidon</t>
-  </si>
-  <si>
-    <t>Swordsaint</t>
-  </si>
-  <si>
-    <t>Wilder</t>
-  </si>
-  <si>
-    <t>Striker/Defender</t>
-  </si>
-  <si>
-    <t>+1 Fortitude, +1 Will</t>
-  </si>
-  <si>
-    <t>Captain</t>
+**Arctic:** You gain the ice stride feature and a +2 bonus to Endure.  
+**Forest or Heath:** You gain the woodland stride feature and a +2 bonus to Nature.  
+**Marshes:** You gain the swamp stride feature and a +2 bonus to Athletics.  
+**Underground or Mountains:** You gain the stone stride feature and a +2 bonus to Dungeoneering.  </t>
+  </si>
+  <si>
+    <t>Arcane Strength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose either Arcane Overflow or Arcane Sustenance. 
+#### Arcane Overflow
+Encounter attack powers from your class disciplines gain the following Miss entry if they do not have one:
+*Miss:* Half damage, and if a hit would have imposed a condition, the target experiences the following (same duration). 
+* *Blinded:* The target is rattled.
+* *Controlled:* The target is dazed.
+* *Immobile:* The target is slowed.
+* *Persistent damage 10 or more:* Persistent damage 5.
+* *Stunned:* The target is dazed.
+* *Weakened:* The target suffers a -4 penalty to damage.
+* *Unwilling movement 3 or more:* Unwilling movement of the same variety 1.
+#### Arcane Sustenance
+At the start of each of your turns, choose one power you have active that requires an action to Maintain or choose a companion of yours (a summon, familiar, etc).
+If you choose the Maintain power, the power is Maintained as if you spent the relevant action on it. If you choose the creature, it can take an action of your choice without you spending an action on it. This does not allow it to exceed its total actions, so for example if you choose for it to take a standard action, you cannot also spend your standard action to have it take another standard action. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You belong to a particular school of magic. Choose one at character creation. 
+* **Conjurer:** When an encounter ends and you have one or more daily powers with the Summon keyword still active, those daily powers are not expended. However, if you use them again, the summoned creatures appear in the exact state they were when their last summoning ended (current HP, conditions, etc) except that they can use their encounter powers again even if already used before. If you complete a long rest, all your daily powers reset and if you use them from then on a "fresh" creature will be summoned. Your secondary ability is Constitution.
+* **Enchanter:** When you use a power with the Psychic tag that does damage on a hit, you can choose for the power to do no damage to any enemies you target. If so, you gain a +2 bonus on the attack roll. Your secondary ability is Charisma. 
+* **Evoker:** If you wish, a Near or Far power you use with the Acid, Cold, Fire, Flux, Lightning or Thunder tags has its area increased by 1 (from Near arc 2 to Near arc 3, for example). Also, you can change your flux energy as a swift action. Your secondary ability is Dexterity. </t>
   </si>
 </sst>
 </file>
@@ -862,13 +884,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1183,10 +1206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB34676-1710-4FA9-B022-445B7CFB73ED}">
-  <dimension ref="A1:AJ18"/>
+  <dimension ref="A1:AL18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18:N18"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AH9" sqref="AH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1201,7 +1224,7 @@
     <col min="14" max="15" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1244,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>219</v>
+        <v>178</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1307,14 +1330,23 @@
       <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="AJ1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>REPT("a",244)</f>
         <v>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</v>
       </c>
       <c r="B2" t="s">
-        <v>218</v>
+        <v>177</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:N2" si="0">REPT("a",244)</f>
@@ -1443,18 +1475,18 @@
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
     </row>
-    <row r="3" spans="1:36" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="E3">
         <v>12</v>
@@ -1463,45 +1495,41 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="H3">
         <v>7</v>
       </c>
       <c r="I3" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="J3" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="K3" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="L3" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="M3"/>
       <c r="N3">
         <v>4</v>
       </c>
       <c r="O3"/>
-      <c r="P3" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>127</v>
-      </c>
+      <c r="P3"/>
+      <c r="Q3" s="3"/>
       <c r="R3" t="s">
-        <v>128</v>
-      </c>
-      <c r="S3" t="s">
-        <v>129</v>
+        <v>97</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="T3" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="V3"/>
       <c r="W3"/>
@@ -1513,32 +1541,40 @@
       <c r="AC3"/>
       <c r="AD3"/>
       <c r="AE3" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="AF3" t="s">
-        <v>132</v>
+        <v>212</v>
       </c>
       <c r="AG3"/>
       <c r="AH3" s="3" t="s">
-        <v>133</v>
+        <v>197</v>
       </c>
       <c r="AI3" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="AJ3"/>
+        <v>100</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>192</v>
+      </c>
+      <c r="AK3" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>100</v>
+      </c>
     </row>
-    <row r="4" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="E4">
         <v>12</v>
@@ -1547,78 +1583,87 @@
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4">
         <v>7</v>
       </c>
       <c r="I4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="J4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="K4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="L4" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="M4" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="N4">
         <v>3</v>
       </c>
       <c r="P4" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="R4" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="S4" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="T4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="U4" t="s">
-        <v>83</v>
+        <v>219</v>
       </c>
       <c r="V4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>199</v>
+      </c>
+      <c r="AL4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>84</v>
-      </c>
-      <c r="W4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AI4" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>105</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -1627,72 +1672,67 @@
         <v>6</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="H5">
         <v>9</v>
       </c>
       <c r="I5" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="J5" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="L5" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="N5">
         <v>3</v>
       </c>
       <c r="P5" t="s">
-        <v>110</v>
+        <v>189</v>
       </c>
       <c r="Q5" t="s">
-        <v>111</v>
-      </c>
-      <c r="R5" t="s">
-        <v>112</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>113</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="S5" s="3"/>
       <c r="T5" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="U5" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="V5" t="s">
-        <v>116</v>
+        <v>221</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>117</v>
+        <v>222</v>
       </c>
       <c r="AE5" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="AF5" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="AH5" s="3" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="AI5" s="3" t="s">
-        <v>121</v>
+        <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -1701,72 +1741,72 @@
         <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6">
         <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="J6" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="K6" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="L6" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="M6" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="N6">
         <v>4</v>
       </c>
       <c r="P6" t="s">
-        <v>95</v>
+        <v>185</v>
       </c>
       <c r="Q6" t="s">
-        <v>96</v>
-      </c>
-      <c r="R6" t="s">
-        <v>97</v>
-      </c>
-      <c r="S6" t="s">
-        <v>98</v>
+        <v>186</v>
       </c>
       <c r="T6" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="U6" t="s">
-        <v>100</v>
+        <v>81</v>
+      </c>
+      <c r="V6" t="s">
+        <v>223</v>
+      </c>
+      <c r="W6" t="s">
+        <v>224</v>
       </c>
       <c r="AE6" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="AF6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
       <c r="AI6" s="3" t="s">
-        <v>104</v>
+        <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E7">
         <v>15</v>
@@ -1775,78 +1815,87 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H7">
         <v>8</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="J7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>227</v>
       </c>
       <c r="L7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="M7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N7">
         <v>3</v>
       </c>
       <c r="P7" t="s">
-        <v>60</v>
+        <v>214</v>
       </c>
       <c r="Q7" t="s">
-        <v>61</v>
+        <v>215</v>
       </c>
       <c r="R7" t="s">
-        <v>62</v>
-      </c>
-      <c r="S7" t="s">
-        <v>63</v>
+        <v>53</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="T7" t="s">
-        <v>64</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
+      </c>
+      <c r="U7" t="s">
+        <v>226</v>
       </c>
       <c r="V7" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="W7" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="AE7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="AF7" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="AH7" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="AI7" s="3" t="s">
-        <v>70</v>
+        <v>216</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>201</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>200</v>
+      </c>
+      <c r="AL7">
+        <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -1855,69 +1904,69 @@
         <v>5</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="H8">
         <v>7</v>
       </c>
       <c r="I8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="J8" t="s">
-        <v>156</v>
+        <v>119</v>
       </c>
       <c r="L8" t="s">
-        <v>157</v>
+        <v>120</v>
       </c>
       <c r="M8" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
       <c r="N8">
         <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>159</v>
+        <v>122</v>
       </c>
       <c r="Q8" t="s">
-        <v>160</v>
+        <v>123</v>
       </c>
       <c r="R8" t="s">
-        <v>161</v>
+        <v>124</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>162</v>
+        <v>217</v>
       </c>
       <c r="T8" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="U8" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="AE8" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
       <c r="AF8" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="AH8" s="3" t="s">
-        <v>165</v>
+        <v>127</v>
       </c>
       <c r="AI8" s="3" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>206</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
         <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -1926,72 +1975,81 @@
         <v>4</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9">
         <v>6</v>
       </c>
       <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" t="s">
         <v>38</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>39</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>40</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>41</v>
-      </c>
-      <c r="M9" t="s">
-        <v>42</v>
       </c>
       <c r="N9">
         <v>3</v>
       </c>
       <c r="P9" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="R9" t="s">
+        <v>42</v>
+      </c>
+      <c r="S9" t="s">
+        <v>219</v>
+      </c>
+      <c r="T9" t="s">
         <v>43</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="U9" t="s">
         <v>44</v>
       </c>
-      <c r="R9" t="s">
+      <c r="AE9" t="s">
         <v>45</v>
       </c>
-      <c r="S9" t="s">
-        <v>46</v>
-      </c>
-      <c r="T9" t="s">
-        <v>47</v>
-      </c>
-      <c r="U9" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>49</v>
-      </c>
       <c r="AF9" t="s">
-        <v>50</v>
+        <v>218</v>
       </c>
       <c r="AH9" s="3" t="s">
-        <v>51</v>
+        <v>232</v>
       </c>
       <c r="AI9" s="3" t="s">
-        <v>52</v>
+        <v>207</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>202</v>
+      </c>
+      <c r="AL9">
+        <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="E10">
         <v>12</v>
@@ -2000,72 +2058,81 @@
         <v>5</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="H10">
         <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="J10" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="L10" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="N10">
         <v>4</v>
       </c>
       <c r="P10" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
       <c r="Q10" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="R10" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="T10" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="U10" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="V10" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="W10" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="AE10" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
       <c r="AF10" t="s">
-        <v>150</v>
+        <v>208</v>
       </c>
       <c r="AH10" s="3" t="s">
-        <v>151</v>
+        <v>228</v>
       </c>
       <c r="AI10" s="3" t="s">
-        <v>152</v>
+        <v>209</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AL10">
+        <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>167</v>
+        <v>129</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>154</v>
+        <v>117</v>
       </c>
       <c r="D11" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="E11">
         <v>12</v>
@@ -2074,63 +2141,63 @@
         <v>5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="H11">
         <v>6</v>
       </c>
       <c r="I11" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="J11" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="K11" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="L11" t="s">
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="M11" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
       <c r="N11">
         <v>3</v>
       </c>
       <c r="P11" t="s">
-        <v>172</v>
+        <v>134</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>173</v>
+        <v>210</v>
       </c>
       <c r="R11" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>175</v>
+        <v>229</v>
       </c>
       <c r="AE11" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
       <c r="AF11" t="s">
-        <v>177</v>
+        <v>137</v>
       </c>
       <c r="AH11" s="3" t="s">
-        <v>178</v>
+        <v>138</v>
       </c>
       <c r="AI11" s="3" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="E12">
         <v>12</v>
@@ -2139,75 +2206,75 @@
         <v>5</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="H12">
         <v>6</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="J12" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="K12" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="L12" t="s">
-        <v>193</v>
+        <v>153</v>
       </c>
       <c r="N12">
         <v>4</v>
       </c>
       <c r="P12" t="s">
-        <v>194</v>
+        <v>154</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
       <c r="R12" t="s">
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="S12" t="s">
-        <v>197</v>
+        <v>157</v>
       </c>
       <c r="T12" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="U12" t="s">
-        <v>199</v>
+        <v>159</v>
       </c>
       <c r="V12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="W12" t="s">
-        <v>83</v>
+        <v>219</v>
       </c>
       <c r="AE12" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="AF12" t="s">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="AG12" t="s">
-        <v>201</v>
+        <v>161</v>
       </c>
       <c r="AH12" s="3" t="s">
-        <v>202</v>
+        <v>162</v>
       </c>
       <c r="AI12" s="3" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>204</v>
+        <v>163</v>
       </c>
       <c r="C13" t="s">
-        <v>205</v>
+        <v>164</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -2216,81 +2283,81 @@
         <v>4</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="H13">
         <v>6</v>
       </c>
       <c r="I13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="J13" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="K13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L13" t="s">
-        <v>206</v>
+        <v>165</v>
       </c>
       <c r="N13">
         <v>4</v>
       </c>
       <c r="P13" t="s">
-        <v>207</v>
+        <v>166</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="R13" t="s">
-        <v>209</v>
+        <v>168</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>210</v>
+        <v>169</v>
       </c>
       <c r="T13" t="s">
+        <v>42</v>
+      </c>
+      <c r="U13" t="s">
+        <v>219</v>
+      </c>
+      <c r="V13" t="s">
+        <v>170</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="X13" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE13" t="s">
         <v>45</v>
       </c>
-      <c r="U13" t="s">
-        <v>83</v>
-      </c>
-      <c r="V13" t="s">
-        <v>211</v>
-      </c>
-      <c r="W13" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="X13" t="s">
-        <v>213</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>214</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>49</v>
-      </c>
       <c r="AF13" t="s">
-        <v>215</v>
+        <v>174</v>
       </c>
       <c r="AG13" t="s">
-        <v>216</v>
+        <v>175</v>
       </c>
       <c r="AH13" t="s">
-        <v>216</v>
+        <v>175</v>
       </c>
       <c r="AI13" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="E14">
         <v>15</v>
@@ -2299,63 +2366,63 @@
         <v>6</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="H14">
         <v>9</v>
       </c>
       <c r="I14" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="J14" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="L14" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="N14">
         <v>4</v>
       </c>
       <c r="P14" t="s">
-        <v>182</v>
+        <v>142</v>
       </c>
       <c r="Q14" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="R14" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
       <c r="S14" t="s">
-        <v>185</v>
+        <v>145</v>
       </c>
       <c r="T14" t="s">
-        <v>186</v>
+        <v>146</v>
       </c>
       <c r="U14" t="s">
-        <v>187</v>
+        <v>147</v>
       </c>
       <c r="V14" t="s">
-        <v>188</v>
+        <v>148</v>
       </c>
       <c r="W14" t="s">
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="AE14" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="AF14" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E15">
         <v>15</v>
@@ -2364,33 +2431,33 @@
         <v>6</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="H15">
         <v>9</v>
       </c>
       <c r="I15" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="J15" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="L15" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="N15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>221</v>
+        <v>180</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="E16">
         <v>12</v>
@@ -2399,19 +2466,19 @@
         <v>5</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="H16">
         <v>6</v>
       </c>
       <c r="I16" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="J16" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="L16" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="N16">
         <v>4</v>
@@ -2419,13 +2486,13 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>222</v>
+        <v>181</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>223</v>
+        <v>182</v>
       </c>
       <c r="E17">
         <v>15</v>
@@ -2434,22 +2501,22 @@
         <v>6</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>224</v>
+        <v>183</v>
       </c>
       <c r="H17">
         <v>8</v>
       </c>
       <c r="I17" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="J17" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="K17" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="L17" t="s">
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="N17">
         <v>4</v>
@@ -2457,13 +2524,13 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>225</v>
+        <v>184</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="E18">
         <v>12</v>
@@ -2472,22 +2539,22 @@
         <v>5</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H18">
         <v>7</v>
       </c>
       <c r="I18" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="J18" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="K18" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="L18" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="N18">
         <v>4</v>
@@ -2499,5 +2566,6 @@
     <sortCondition ref="A3:A56"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding the Warrior class, the Weapon Drill discipline, and updating shapechanging to be more fun
</commit_message>
<xml_diff>
--- a/data/Orcus - Classes.xlsx
+++ b/data/Orcus - Classes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Obsidian\Tabletop games\d20 System or D&amp;D-esque\2021 Orcus - 4E clone\GitHub\orcus\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21DD73B-FF31-4A56-874D-0120D09DE39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C93BB7E-B3D9-4ADD-8090-FC952A77D44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{190BB917-E992-4FE1-9680-9C1683F26666}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="244">
   <si>
     <t>Name</t>
   </si>
@@ -339,10 +339,6 @@
 * Proficiency with two exotic melee weapons of your choice. </t>
   </si>
   <si>
-    <t xml:space="preserve">You belong to the Commander class (along with any other classes that you belong to), and gain the following benefits:
-* You can use *lifting words* once per encounter. </t>
-  </si>
-  <si>
     <t>Striker</t>
   </si>
   <si>
@@ -640,9 +636,6 @@
   </si>
   <si>
     <t>pics\Vera.png</t>
-  </si>
-  <si>
-    <t>Vera by Justin Nichols</t>
   </si>
   <si>
     <t>pics\Flashing Ray Color.png</t>
@@ -828,6 +821,61 @@
   </si>
   <si>
     <t xml:space="preserve">You have access to psi focus, a heightened state of mental and emotional clarity, that you can utilize to augment powers with the Augmentable keyword. This psi focus, once used, must refresh, much like how certain monsters have powers that refresh at the beginning of their turn on a successful roll. Psi focus works in the exact same way, refreshing on a roll of 5 or 6.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You belong to the Commander class (along with any other classes that you belong to), and gain the following benefits:
+* You can use *lift spirits* once per encounter. </t>
+  </si>
+  <si>
+    <t>Vera by Justin Nichol</t>
+  </si>
+  <si>
+    <t>Ranger by Justin Nichol</t>
+  </si>
+  <si>
+    <t>pics\Ranger.png</t>
+  </si>
+  <si>
+    <t>Warrior</t>
+  </si>
+  <si>
+    <t>Cloth, leather, hide, chainmail, scale; light shield</t>
+  </si>
+  <si>
+    <t>Bonus Feat</t>
+  </si>
+  <si>
+    <t>Bear and Wolf Styles</t>
+  </si>
+  <si>
+    <t>When your hit points are high enough that you are not staggered, you have the Bear Style feature. While you are staggered, you lose Bear Style and gain the Wolf Style feature until you are healed enough that you are no longer Staggered.
+*Bear Style:* Adjacent enemies suffer a -2 penalty to attacks that do not include you as a target, unless they have the marked condition.
+*Wolf Style:* Once per round, you can do additional damage when you hit with an attack. *Level 1:* +1d8. *Level 11:* +2d8. *Level 21:* +3d8.</t>
+  </si>
+  <si>
+    <t>Warrior Powers</t>
+  </si>
+  <si>
+    <t>Fatigue Points</t>
+  </si>
+  <si>
+    <t>Multiclassing, Kits and Other Power Swaps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characters in *Orcus* often replace class powers with other powers. The warrior can do so under the same circumstances, but they lose one Focus Point for every power that they do so with. For example, a Warrior with the Dabbles in Wizardry kit could take *cut the strings* as a level 3 encounter power. If so, they would lose one Fatigue Point, but could use *cut the strings* once an encounter (not requiring them to spend any Fatigue Points). </t>
+  </si>
+  <si>
+    <t>You gain one of the following feats of your choice: Armor Proficiency, Shield Proficiency, Two-Weapon Defense, Unarmed Combat or Weapon Proficiency.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At level 1, you have 1 Fatigue Point. You gain an additional Fatigue Point at levels 3, 7 and 9. You can spend one Fatigue Point to use any encounter attack power you have learned via Warrior Power. After a short rest, you recover all spent Fatigue Points. 
+You can also use any daily attack power that you know, but it takes time to set these powers up. You must declare that you are using the daily power on your turn, and spend a Fatigue Point. On your next turn, you must use that power. If you are no longer able to do so or no longer want to use the power, for that turn you lose whatever action that power would have taken and the Fatigue Point remains spent.
+The normal limit that an encounter power can only be used once between short rests and a daily power once between long rests do not apply to your class attack powers. However, you cannot use any daily attack power more than once an encounter. </t>
+  </si>
+  <si>
+    <t>As a warrior, you learn and use powers differently to other classes. You know all at-will powers in the Weapon Drill discipline, and can use them as normal at-will powers. These replace the two level 1 at-will attack powers that other heroes gain at level 1. 
+From level 1, you also know two level 1 attack powers (encounter or daily, or one of each) from any martial discipline. At levels 3, 5, 7, 9, 13, 15, 19, 23, 25 and 29, you learn an additional attack power (encounter or daily) of your level or lower from any martial discipline. These are your class attack powers. However, you cannot use these powers without spending Fatigue Points (see below). 
+You learn utility powers as normal.</t>
   </si>
 </sst>
 </file>
@@ -1193,13 +1241,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB34676-1710-4FA9-B022-445B7CFB73ED}">
-  <dimension ref="A1:AL18"/>
+  <dimension ref="A1:AL19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1234,7 +1282,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1321,13 +1369,13 @@
         <v>33</v>
       </c>
       <c r="AJ1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="AK1" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="AL1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1510,7 +1558,7 @@
         <v>92</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T3" t="s">
         <v>93</v>
@@ -1522,19 +1570,19 @@
         <v>79</v>
       </c>
       <c r="AF3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AI3" s="3" t="s">
-        <v>95</v>
+        <v>228</v>
       </c>
       <c r="AJ3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AK3" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AL3" s="1">
         <v>100</v>
@@ -1600,7 +1648,7 @@
         <v>42</v>
       </c>
       <c r="U4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="V4" t="s">
         <v>70</v>
@@ -1619,7 +1667,7 @@
         <v>72</v>
       </c>
       <c r="AF4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="AG4"/>
       <c r="AH4" s="3" t="s">
@@ -1629,10 +1677,10 @@
         <v>74</v>
       </c>
       <c r="AJ4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AK4" t="s">
         <v>185</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>186</v>
       </c>
       <c r="AL4">
         <v>25</v>
@@ -1640,7 +1688,7 @@
     </row>
     <row r="5" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1649,7 +1697,7 @@
         <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -1658,64 +1706,64 @@
         <v>5</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H5">
         <v>6</v>
       </c>
       <c r="I5" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" t="s">
         <v>98</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>99</v>
-      </c>
-      <c r="L5" t="s">
-        <v>100</v>
       </c>
       <c r="N5">
         <v>4</v>
       </c>
       <c r="P5" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q5" t="s">
         <v>101</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>102</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="T5" t="s">
         <v>103</v>
       </c>
-      <c r="S5" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>104</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>105</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>106</v>
       </c>
-      <c r="W5" t="s">
+      <c r="AE5" t="s">
         <v>107</v>
       </c>
-      <c r="AE5" t="s">
-        <v>108</v>
-      </c>
       <c r="AF5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AH5" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AI5" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AJ5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AK5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AL5">
         <v>20</v>
@@ -1723,7 +1771,7 @@
     </row>
     <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1759,10 +1807,10 @@
         <v>3</v>
       </c>
       <c r="P6" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q6" t="s">
         <v>176</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>177</v>
       </c>
       <c r="S6" s="3"/>
       <c r="T6" t="s">
@@ -1772,10 +1820,10 @@
         <v>85</v>
       </c>
       <c r="V6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="AE6" t="s">
         <v>86</v>
@@ -1787,12 +1835,12 @@
         <v>88</v>
       </c>
       <c r="AI6" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1834,28 +1882,28 @@
         <v>4</v>
       </c>
       <c r="P7" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q7" t="s">
         <v>173</v>
       </c>
-      <c r="Q7" t="s">
-        <v>174</v>
-      </c>
       <c r="V7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="W7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AE7" t="s">
         <v>79</v>
       </c>
       <c r="AF7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AH7" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AI7" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1890,7 +1938,7 @@
         <v>50</v>
       </c>
       <c r="K8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L8" t="s">
         <v>51</v>
@@ -1902,10 +1950,10 @@
         <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="Q8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="R8" t="s">
         <v>53</v>
@@ -1917,13 +1965,13 @@
         <v>52</v>
       </c>
       <c r="U8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="V8" t="s">
         <v>55</v>
       </c>
       <c r="W8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AE8" t="s">
         <v>45</v>
@@ -1935,13 +1983,13 @@
         <v>57</v>
       </c>
       <c r="AI8" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AJ8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AK8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AL8">
         <v>20</v>
@@ -1949,7 +1997,7 @@
     </row>
     <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1991,16 +2039,16 @@
         <v>3</v>
       </c>
       <c r="P9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="R9" t="s">
         <v>42</v>
       </c>
       <c r="S9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="T9" t="s">
         <v>43</v>
@@ -2012,19 +2060,19 @@
         <v>45</v>
       </c>
       <c r="AF9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AH9" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AI9" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AJ9" t="s">
-        <v>190</v>
+        <v>229</v>
       </c>
       <c r="AK9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AL9">
         <v>25</v>
@@ -2032,13 +2080,13 @@
     </row>
     <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
         <v>35</v>
@@ -2050,7 +2098,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H10">
         <v>7</v>
@@ -2059,60 +2107,66 @@
         <v>49</v>
       </c>
       <c r="J10" t="s">
+        <v>111</v>
+      </c>
+      <c r="L10" t="s">
         <v>112</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>113</v>
-      </c>
-      <c r="M10" t="s">
-        <v>114</v>
       </c>
       <c r="N10">
         <v>3</v>
       </c>
       <c r="P10" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q10" t="s">
         <v>115</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>116</v>
       </c>
-      <c r="R10" t="s">
-        <v>117</v>
-      </c>
       <c r="S10" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="T10" t="s">
         <v>70</v>
       </c>
       <c r="U10" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>224</v>
+      </c>
+      <c r="AH10" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AI10" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="AE10" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>226</v>
-      </c>
-      <c r="AH10" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="AI10" s="3" t="s">
-        <v>119</v>
+      <c r="AJ10" t="s">
+        <v>230</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E11">
         <v>12</v>
@@ -2121,57 +2175,57 @@
         <v>5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H11">
         <v>6</v>
       </c>
       <c r="I11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J11" t="s">
         <v>82</v>
       </c>
       <c r="K11" t="s">
+        <v>122</v>
+      </c>
+      <c r="L11" t="s">
         <v>123</v>
       </c>
-      <c r="L11" t="s">
-        <v>124</v>
-      </c>
       <c r="M11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N11">
         <v>3</v>
       </c>
       <c r="P11" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="R11" t="s">
         <v>125</v>
       </c>
-      <c r="Q11" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="R11" t="s">
+      <c r="S11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AE11" t="s">
         <v>126</v>
       </c>
-      <c r="S11" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="AE11" t="s">
+      <c r="AF11" t="s">
         <v>127</v>
       </c>
-      <c r="AF11" t="s">
+      <c r="AH11" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="AH11" s="3" t="s">
+      <c r="AI11" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="AI11" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C12" t="s">
         <v>75</v>
@@ -2209,13 +2263,13 @@
     </row>
     <row r="13" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E13">
         <v>12</v>
@@ -2224,7 +2278,7 @@
         <v>5</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H13">
         <v>6</v>
@@ -2236,57 +2290,57 @@
         <v>62</v>
       </c>
       <c r="K13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N13">
         <v>4</v>
       </c>
       <c r="P13" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q13" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="Q13" s="3" t="s">
+      <c r="R13" t="s">
         <v>146</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>147</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>148</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>149</v>
-      </c>
-      <c r="U13" t="s">
-        <v>150</v>
       </c>
       <c r="V13" t="s">
         <v>42</v>
       </c>
       <c r="W13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="AE13" t="s">
         <v>79</v>
       </c>
       <c r="AF13" t="s">
+        <v>150</v>
+      </c>
+      <c r="AG13" t="s">
         <v>151</v>
       </c>
-      <c r="AG13" t="s">
+      <c r="AH13" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="AH13" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="AI13" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C14" t="s">
         <v>75</v>
@@ -2321,10 +2375,10 @@
     </row>
     <row r="15" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" t="s">
         <v>154</v>
-      </c>
-      <c r="C15" t="s">
-        <v>155</v>
       </c>
       <c r="D15" t="s">
         <v>35</v>
@@ -2336,7 +2390,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H15">
         <v>6</v>
@@ -2351,66 +2405,66 @@
         <v>39</v>
       </c>
       <c r="L15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N15">
         <v>4</v>
       </c>
       <c r="P15" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q15" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="Q15" s="3" t="s">
+      <c r="R15" t="s">
         <v>158</v>
       </c>
-      <c r="R15" t="s">
-        <v>159</v>
-      </c>
       <c r="S15" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="T15" t="s">
         <v>42</v>
       </c>
       <c r="U15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="V15" t="s">
+        <v>159</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="X15" t="s">
         <v>160</v>
       </c>
-      <c r="W15" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>161</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>162</v>
       </c>
       <c r="AE15" t="s">
         <v>45</v>
       </c>
       <c r="AF15" t="s">
+        <v>162</v>
+      </c>
+      <c r="AG15" t="s">
         <v>163</v>
       </c>
-      <c r="AG15" t="s">
+      <c r="AH15" t="s">
+        <v>163</v>
+      </c>
+      <c r="AI15" t="s">
         <v>164</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>164</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C16" t="s">
         <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E16">
         <v>12</v>
@@ -2419,19 +2473,19 @@
         <v>5</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H16">
         <v>6</v>
       </c>
       <c r="I16" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" t="s">
         <v>98</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>99</v>
-      </c>
-      <c r="L16" t="s">
-        <v>100</v>
       </c>
       <c r="N16">
         <v>4</v>
@@ -2439,13 +2493,13 @@
     </row>
     <row r="17" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
         <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E17">
         <v>15</v>
@@ -2454,13 +2508,13 @@
         <v>6</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H17">
         <v>9</v>
       </c>
       <c r="I17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J17" t="s">
         <v>82</v>
@@ -2472,45 +2526,45 @@
         <v>4</v>
       </c>
       <c r="P17" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q17" t="s">
         <v>133</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>134</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>135</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>136</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>137</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>138</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>139</v>
-      </c>
-      <c r="W17" t="s">
-        <v>140</v>
       </c>
       <c r="AE17" t="s">
         <v>86</v>
       </c>
       <c r="AF17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C18" t="s">
         <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E18">
         <v>15</v>
@@ -2519,25 +2573,96 @@
         <v>6</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H18">
         <v>8</v>
       </c>
       <c r="I18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J18" t="s">
         <v>82</v>
       </c>
       <c r="K18" t="s">
+        <v>122</v>
+      </c>
+      <c r="L18" t="s">
         <v>123</v>
-      </c>
-      <c r="L18" t="s">
-        <v>124</v>
       </c>
       <c r="N18">
         <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="I19" t="s">
+        <v>233</v>
+      </c>
+      <c r="J19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K19" t="s">
+        <v>122</v>
+      </c>
+      <c r="L19" t="s">
+        <v>123</v>
+      </c>
+      <c r="N19">
+        <v>4</v>
+      </c>
+      <c r="P19" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>241</v>
+      </c>
+      <c r="R19" t="s">
+        <v>235</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="T19" t="s">
+        <v>237</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="V19" t="s">
+        <v>238</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="X19" t="s">
+        <v>239</v>
+      </c>
+      <c r="Y19" s="3" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>